<commit_message>
REVISION VERSION, submitted Sc5 run 07/2020
</commit_message>
<xml_diff>
--- a/data for modeling_updated 30June2020_withPolynomialCoefficients.xlsx
+++ b/data for modeling_updated 30June2020_withPolynomialCoefficients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MyDesk/Dropbox/From_iCloud/ONGOING PROJECTS/Adina/StableStrontium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0FAAC7B-CA10-DD49-8DAF-81C91ED4C73B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E9CAC4-36EC-C74F-90F6-003DE7E89D12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="780" windowWidth="26020" windowHeight="12700" activeTab="1" xr2:uid="{0973490E-C09A-C249-B219-928F56E66B8A}"/>
+    <workbookView xWindow="7940" yWindow="10500" windowWidth="26020" windowHeight="12700" activeTab="1" xr2:uid="{0973490E-C09A-C249-B219-928F56E66B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="full data set" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="143">
   <si>
     <t>Site</t>
   </si>
@@ -500,6 +500,30 @@
   </si>
   <si>
     <t>Sc5</t>
+  </si>
+  <si>
+    <t>X^0</t>
+  </si>
+  <si>
+    <t>X^1</t>
+  </si>
+  <si>
+    <t>X^7</t>
+  </si>
+  <si>
+    <t>X^6</t>
+  </si>
+  <si>
+    <t>X^5</t>
+  </si>
+  <si>
+    <t>X^4</t>
+  </si>
+  <si>
+    <t>X^3</t>
+  </si>
+  <si>
+    <t>X^2</t>
   </si>
 </sst>
 </file>
@@ -13435,7 +13459,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13464,6 +13488,9 @@
       <c r="A2" t="s">
         <v>124</v>
       </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
       <c r="D2" s="49">
         <v>-6.9223939587266197E-10</v>
       </c>
@@ -13484,6 +13511,9 @@
       <c r="A3" t="s">
         <v>125</v>
       </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
       <c r="D3" s="49">
         <v>9.0534222621938593E-8</v>
       </c>
@@ -13504,6 +13534,9 @@
       <c r="A4" t="s">
         <v>127</v>
       </c>
+      <c r="C4" t="s">
+        <v>139</v>
+      </c>
       <c r="D4" s="49">
         <v>-4.6861368980428401E-6</v>
       </c>
@@ -13524,6 +13557,9 @@
       <c r="A5" t="s">
         <v>128</v>
       </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
       <c r="D5" s="49">
         <v>1.21100069135726E-4</v>
       </c>
@@ -13544,6 +13580,9 @@
       <c r="A6" t="s">
         <v>126</v>
       </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
       <c r="D6" s="49">
         <v>-1.60373266265369E-3</v>
       </c>
@@ -13561,6 +13600,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
       <c r="D7" s="49">
         <v>9.8169958785834996E-3</v>
       </c>
@@ -13578,6 +13620,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>136</v>
+      </c>
       <c r="D8" s="49">
         <v>-2.03003298040779E-2</v>
       </c>
@@ -13595,6 +13640,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
       <c r="D9" s="49">
         <v>0.354751635919481</v>
       </c>

</xml_diff>